<commit_message>
integration changes and upgrade db
</commit_message>
<xml_diff>
--- a/GDD AOE2 Cards.xlsx
+++ b/GDD AOE2 Cards.xlsx
@@ -300,9 +300,6 @@
     <t>Teutons</t>
   </si>
   <si>
-    <t>Teutons Resistance</t>
-  </si>
-  <si>
     <t>Vietnamese</t>
   </si>
   <si>
@@ -559,6 +556,9 @@
   </si>
   <si>
     <t>Camels +4</t>
+  </si>
+  <si>
+    <t>Teutons Faith</t>
   </si>
 </sst>
 </file>
@@ -5616,8 +5616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5635,16 +5635,16 @@
         <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" t="s">
-        <v>136</v>
-      </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -5664,7 +5664,7 @@
         <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5675,13 +5675,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5692,7 +5692,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -5706,7 +5706,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -5720,7 +5720,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -5734,7 +5734,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -5748,7 +5748,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -5776,7 +5776,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -5793,7 +5793,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -5810,7 +5810,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -5827,7 +5827,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -5858,7 +5858,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15">
         <v>13</v>
@@ -5872,7 +5872,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16">
         <v>12</v>
@@ -5900,7 +5900,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18">
         <v>14</v>
@@ -5914,7 +5914,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19">
         <v>15</v>
@@ -5925,13 +5925,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20">
         <v>15</v>
@@ -5948,7 +5948,7 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D21">
         <v>15</v>
@@ -5965,7 +5965,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22">
         <v>16</v>
@@ -5979,7 +5979,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23">
         <v>17</v>
@@ -6007,7 +6007,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25">
         <v>18</v>
@@ -6035,7 +6035,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27">
         <v>20</v>
@@ -6049,7 +6049,7 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D28">
         <v>21</v>
@@ -6063,7 +6063,7 @@
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29">
         <v>22</v>
@@ -6077,7 +6077,7 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D30">
         <v>23</v>
@@ -6105,7 +6105,7 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D32">
         <v>25</v>
@@ -6119,7 +6119,7 @@
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -6136,7 +6136,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -6153,7 +6153,7 @@
         <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -6167,19 +6167,19 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
         <v>135</v>
       </c>
-      <c r="C37" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" t="s">
-        <v>136</v>
-      </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -6193,13 +6193,13 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E38">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -6219,7 +6219,7 @@
         <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -6239,7 +6239,7 @@
         <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6253,18 +6253,18 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
       <c r="F41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
@@ -6273,13 +6273,13 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E42">
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -6299,7 +6299,7 @@
         <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -6319,7 +6319,7 @@
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -6402,7 +6402,7 @@
         <v>68</v>
       </c>
       <c r="J48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -6425,7 +6425,7 @@
         <v>71</v>
       </c>
       <c r="I49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J49">
         <f>(D2+E39+E40+E41+E42)*E38</f>
@@ -6434,22 +6434,25 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
         <v>120</v>
       </c>
-      <c r="F50" t="s">
-        <v>121</v>
-      </c>
       <c r="I50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J50">
         <f>D27+E44+E46+E47+E48+E45</f>
@@ -6458,22 +6461,25 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D51" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
         <v>123</v>
       </c>
-      <c r="F51" t="s">
-        <v>124</v>
-      </c>
       <c r="I51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J51">
         <f>D24+E67+E68+E69+E70+E72</f>
@@ -6488,7 +6494,7 @@
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D52" t="s">
         <v>74</v>
@@ -6497,7 +6503,7 @@
         <v>4</v>
       </c>
       <c r="F52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -6508,7 +6514,7 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D53" t="s">
         <v>87</v>
@@ -6517,10 +6523,10 @@
         <v>6</v>
       </c>
       <c r="F53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J53">
         <f>D31+E59+E60+E62+E64</f>
@@ -6529,25 +6535,25 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E54">
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J54">
         <f>D28+E65+E62+E60+E66+E64</f>
@@ -6556,25 +6562,25 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
         <v>125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" t="s">
-        <v>126</v>
       </c>
       <c r="E55">
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J55">
         <f>D32+E54+E53+E52+E60+E62</f>
@@ -6583,27 +6589,27 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" t="s">
         <v>128</v>
-      </c>
-      <c r="B56" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" t="s">
-        <v>165</v>
-      </c>
-      <c r="D56" t="s">
-        <v>129</v>
       </c>
       <c r="E56">
         <v>4</v>
       </c>
       <c r="F56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
         <v>2</v>
@@ -6612,18 +6618,18 @@
         <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E57">
         <v>6</v>
       </c>
       <c r="F57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B58" t="s">
         <v>2</v>
@@ -6632,13 +6638,13 @@
         <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E58">
         <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -6732,15 +6738,18 @@
         <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>94</v>
+        <v>180</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -6749,7 +6758,7 @@
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E64">
         <v>4</v>
@@ -6766,7 +6775,7 @@
         <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D65" t="s">
         <v>85</v>
@@ -6775,7 +6784,7 @@
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6786,7 +6795,7 @@
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D66" t="s">
         <v>92</v>
@@ -6795,12 +6804,12 @@
         <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
@@ -6809,18 +6818,18 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E67">
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
         <v>2</v>
@@ -6829,18 +6838,18 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E68">
         <v>4</v>
       </c>
       <c r="F68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
@@ -6849,18 +6858,18 @@
         <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E69">
         <v>6</v>
       </c>
       <c r="F69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
         <v>2</v>
@@ -6869,18 +6878,18 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E70">
         <v>6</v>
       </c>
       <c r="F70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
@@ -6889,18 +6898,18 @@
         <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E71">
         <v>4</v>
       </c>
       <c r="F71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B72" t="s">
         <v>2</v>
@@ -6909,18 +6918,18 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E72">
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some rename of images and add arclayout for hand cards
</commit_message>
<xml_diff>
--- a/GDD AOE2 Cards.xlsx
+++ b/GDD AOE2 Cards.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="18855" windowHeight="6150"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="18855" windowHeight="6150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$N$1:$O$11</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="229">
   <si>
     <t>Villager</t>
   </si>
@@ -559,13 +562,157 @@
   </si>
   <si>
     <t>Teutons Faith</t>
+  </si>
+  <si>
+    <t>Infantry</t>
+  </si>
+  <si>
+    <t>Infantry|Counter Unit</t>
+  </si>
+  <si>
+    <t>Cavalry</t>
+  </si>
+  <si>
+    <t>Cavalry|Counter Unit</t>
+  </si>
+  <si>
+    <t>Infantry|Militia</t>
+  </si>
+  <si>
+    <t>Eagle Scout</t>
+  </si>
+  <si>
+    <t>Infantry|Eagle Warrior</t>
+  </si>
+  <si>
+    <t>+5 vs Infantry</t>
+  </si>
+  <si>
+    <t>+5 vs Cavalry</t>
+  </si>
+  <si>
+    <t>Light Cavalry</t>
+  </si>
+  <si>
+    <t>+5 vs Archer</t>
+  </si>
+  <si>
+    <t>Long Swordsman</t>
+  </si>
+  <si>
+    <t>Cavalry Archer</t>
+  </si>
+  <si>
+    <t>Archer | Cavalry</t>
+  </si>
+  <si>
+    <t>Archer|Cavalry|Cavalry Archer</t>
+  </si>
+  <si>
+    <t>Cavalry|Camel</t>
+  </si>
+  <si>
+    <t>+6 vs Cavalry</t>
+  </si>
+  <si>
+    <t>+6 vs Infantry</t>
+  </si>
+  <si>
+    <t>Archer|Infantry</t>
+  </si>
+  <si>
+    <t>Cavalry|Elephant</t>
+  </si>
+  <si>
+    <t>Always wins vs Cavalry</t>
+  </si>
+  <si>
+    <t>Siege Ram</t>
+  </si>
+  <si>
+    <t>Heavy Scorpion</t>
+  </si>
+  <si>
+    <t>Always wins vs Infantry</t>
+  </si>
+  <si>
+    <t>Base Power</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Archetypes</t>
+  </si>
+  <si>
+    <t>Vs Unit Effect</t>
+  </si>
+  <si>
+    <t>Effect Power</t>
+  </si>
+  <si>
+    <t>Infantry +8</t>
+  </si>
+  <si>
+    <t>Infantry +8 vs Archers</t>
+  </si>
+  <si>
+    <t>Infantry +4</t>
+  </si>
+  <si>
+    <t>Japanese Warriors</t>
+  </si>
+  <si>
+    <t>Infantry +8 vs Infantry</t>
+  </si>
+  <si>
+    <t>Infantry +8 vs Cavalry</t>
+  </si>
+  <si>
+    <t>Elephants +6,</t>
+  </si>
+  <si>
+    <t>Cavalry Archer|Counter Unit</t>
+  </si>
+  <si>
+    <t>Archers+6(Cavalry Archers)</t>
+  </si>
+  <si>
+    <t>Archers+8(Cavalry Archers)</t>
+  </si>
+  <si>
+    <t>Cavalry +4 vs Infantry</t>
+  </si>
+  <si>
+    <t>Cavalry+4</t>
+  </si>
+  <si>
+    <t>Cavalry +4 vs Archers</t>
+  </si>
+  <si>
+    <t>Cavalry +4</t>
+  </si>
+  <si>
+    <t>Cavalry no longer loses vs monks</t>
+  </si>
+  <si>
+    <t>Archers +4 vs Infantry</t>
+  </si>
+  <si>
+    <t>Archers +4(Cavalry Archers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Villager </t>
+  </si>
+  <si>
+    <t>Counter Unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,16 +720,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -590,12 +751,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,6 +806,252 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Units</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja2!$K$2:$K$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Archer</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camel</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cavalry</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cavalry Archer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Counter Unit</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Eagle Warrior</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Elephant</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Infantry</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Militia</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Monk</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Siege</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Villager </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$L$2:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Upgrades</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja2!$N$2:$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Archer</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camel</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cavalry</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cavalry Archer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Counter Units</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Eagle Warrior</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Elephant</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Infantry</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Infantry</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Monk</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Siege</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Villager</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$O$2:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="108638976"/>
+        <c:axId val="87249280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="108638976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87249280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="87249280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108638976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -5279,6 +5726,116 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="3619500"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 35" descr="KnightIcon">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6667500"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 36" descr="CavalierIcon">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6886575"/>
           <a:ext cx="209550" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5616,8 +6173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6945,30 +7502,1612 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>183</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>183</v>
+      </c>
+      <c r="R4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>193</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>193</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>228</v>
+      </c>
+      <c r="L6">
+        <v>9</v>
+      </c>
+      <c r="N6" t="s">
+        <v>155</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>166</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>166</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>181</v>
+      </c>
+      <c r="L9">
+        <v>12</v>
+      </c>
+      <c r="N9" t="s">
+        <v>181</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>181</v>
+      </c>
+      <c r="R9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
+        <v>181</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>137</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>137</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>137</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>227</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>227</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" t="s">
+        <v>183</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25">
+        <v>18</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27">
+        <v>20</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28">
+        <v>21</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D29">
+        <v>22</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31">
+        <v>24</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C32" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>25</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>201</v>
+      </c>
+      <c r="F33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>204</v>
+      </c>
+      <c r="F35" t="s">
+        <v>181</v>
+      </c>
+      <c r="G35">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="N1:O11">
+    <sortState ref="N2:O13">
+      <sortCondition ref="N1:N11"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>181</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>